<commit_message>
UPDATE ADD _ ANSIBLE _ ROLE
</commit_message>
<xml_diff>
--- a/tEPCRUNNING/server_info.xlsx
+++ b/tEPCRUNNING/server_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="74">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -229,6 +229,36 @@
   </si>
   <si>
     <t xml:space="preserve">COMPUTE14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percona db → false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waite time → pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log docker → failse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looix rabbitmq voi lenh echo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">haproxy thieu sysctl -p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deployment va service setup index  → tran queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thieu mkdir nova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openvswitch and eno2 bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clean skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add ansible service </t>
   </si>
 </sst>
 </file>
@@ -667,10 +697,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1296,6 +1326,86 @@
         <v>37</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="K11:P11"/>

</xml_diff>